<commit_message>
[IMP] forlife_hr_payroll: thêm thông tin đánh dấu TC trên phiếu lương
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_hr_payroll/static/xlsx/template_import_salary_record.xlsx
+++ b/addons/custom/forlife_hr_payroll/static/xlsx/template_import_salary_record.xlsx
@@ -22,6 +22,30 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Nếu là TC thì nhập TC, nếu không thì để trống</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -135,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="93">
   <si>
     <t xml:space="preserve">Loại</t>
   </si>
@@ -147,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mô tả</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC</t>
   </si>
   <si>
     <t xml:space="preserve">4-Sản xuất</t>
@@ -2569,13 +2596,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
@@ -2583,7 +2610,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2596,10 +2623,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2022</v>
@@ -2608,7 +2638,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2625,6 +2658,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2652,36 +2686,36 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="13" t="n">
@@ -2690,16 +2724,16 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="13" t="n">
@@ -2708,16 +2742,16 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="13" t="n">
@@ -2726,16 +2760,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="13" t="n">
@@ -2744,16 +2778,16 @@
     </row>
     <row r="6" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="13" t="n">
@@ -2762,16 +2796,16 @@
     </row>
     <row r="7" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="13" t="n">
@@ -2780,16 +2814,16 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13" t="n">
@@ -2920,7 +2954,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.78"/>
@@ -2932,45 +2966,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -2979,21 +3013,21 @@
         <v>53000000</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -3002,21 +3036,21 @@
         <v>54000000</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -3025,121 +3059,121 @@
         <v>55000000</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="13" t="n">
         <v>56000000</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="13" t="n">
         <v>57000000</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="13" t="n">
         <v>58000000</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="13" t="n">
         <v>59000000</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -3148,18 +3182,18 @@
         <v>60000000</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="19" t="n">
         <v>1401100404</v>
@@ -3171,7 +3205,7 @@
         <v>61000000</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3323,7 +3357,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.78"/>
@@ -3344,78 +3378,78 @@
   <sheetData>
     <row r="1" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -3459,21 +3493,21 @@
         <v>2200000</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -3517,21 +3551,21 @@
         <v>2300000</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -3575,25 +3609,25 @@
         <v>2400000</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="13" t="n">
@@ -3635,25 +3669,25 @@
         <v>2500000</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="13" t="n">
@@ -3695,26 +3729,26 @@
         <v>2600000</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" s="13" t="n">
         <v>9000000</v>
@@ -3755,26 +3789,26 @@
         <v>2700000</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="13" t="n">
         <v>9500000</v>
@@ -3815,21 +3849,21 @@
         <v>2800000</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -3873,21 +3907,21 @@
         <v>2900000</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="14"/>
@@ -3931,7 +3965,7 @@
         <v>3000000</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4072,7 +4106,7 @@
       <selection pane="topRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22"/>
@@ -4094,99 +4128,99 @@
   <sheetData>
     <row r="1" s="34" customFormat="true" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P1" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T1" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="U1" s="32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="V1" s="32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="W1" s="32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X1" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Y1" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="35" t="n">
         <v>107759</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -4237,27 +4271,27 @@
         <v>2600000</v>
       </c>
       <c r="Y2" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="35" t="n">
         <v>107882</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4308,27 +4342,27 @@
         <v>2700000</v>
       </c>
       <c r="Y3" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="35" t="n">
         <v>108005</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -4379,27 +4413,27 @@
         <v>2800000</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="35" t="n">
         <v>108128</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -4450,27 +4484,27 @@
         <v>2900000</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="35" t="n">
         <v>108497</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -4521,27 +4555,27 @@
         <v>3000000</v>
       </c>
       <c r="Y6" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="35" t="n">
         <v>108620</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -4592,27 +4626,27 @@
         <v>3100000</v>
       </c>
       <c r="Y7" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="35" t="n">
         <v>108743</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="14"/>
@@ -4663,7 +4697,7 @@
         <v>3200000</v>
       </c>
       <c r="Y8" s="37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,7 +4868,7 @@
       <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11"/>
@@ -4845,22 +4879,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G1" s="43" t="s">
         <v>2</v>
@@ -4874,19 +4908,19 @@
         <v>107759</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="45" t="n">
         <v>3500000</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,19 +4931,19 @@
         <v>107882</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="45" t="n">
         <v>3600000</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4920,19 +4954,19 @@
         <v>108005</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="45" t="n">
         <v>3700000</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4943,19 +4977,19 @@
         <v>108128</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="45" t="n">
         <v>3800000</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4966,19 +5000,19 @@
         <v>108497</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="45" t="n">
         <v>3900000</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4989,19 +5023,19 @@
         <v>108620</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="45" t="n">
         <v>4000000</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] forlife_hr_payroll: thêm trường phòng ban phụ trách trên bản ghi lương
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_hr_payroll/static/xlsx/template_import_salary_record.xlsx
+++ b/addons/custom/forlife_hr_payroll/static/xlsx/template_import_salary_record.xlsx
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="95">
   <si>
     <t xml:space="preserve">Loại</t>
   </si>
@@ -176,12 +176,24 @@
     <t xml:space="preserve">TC</t>
   </si>
   <si>
+    <t xml:space="preserve">Mã phòng/bp phụ trách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên phòng/bp phụ trách</t>
+  </si>
+  <si>
     <t xml:space="preserve">4-Sản xuất</t>
   </si>
   <si>
     <t xml:space="preserve">hach toan t11.2022</t>
   </si>
   <si>
+    <t xml:space="preserve">PH001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng Hành Chính tổng hợp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mục đích tính lương</t>
   </si>
   <si>
@@ -213,12 +225,6 @@
   </si>
   <si>
     <t xml:space="preserve">6421-Chi phí quản lý doanh nghiệp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng Hành Chính tổng hợp</t>
   </si>
   <si>
     <t xml:space="preserve">1401100409</t>
@@ -669,6 +675,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -695,14 +709,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2596,10 +2602,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2608,6 +2614,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,10 +2634,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2022</v>
@@ -2638,13 +2652,31 @@
         <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2" type="none">
       <formula1>0</formula1>
@@ -2670,124 +2702,124 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="44.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="55.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="4" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="44.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="55.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="6" width="9.11"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="7" t="s">
+    <row r="1" s="10" customFormat="true" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>19</v>
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="E3" s="4"/>
       <c r="F3" s="13" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>29</v>
+      <c r="A6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="13" t="n">
@@ -2795,17 +2827,17 @@
       </c>
     </row>
     <row r="7" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>32</v>
+      <c r="A7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="13" t="n">
@@ -2813,17 +2845,17 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>36</v>
+      <c r="A8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13" t="n">
@@ -2832,85 +2864,85 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
+    <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 B8:C8">
-    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
+    <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C7">
-    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5"/>
+    <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6"/>
+    <cfRule type="duplicateValues" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+    <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
+    <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9"/>
+    <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10"/>
+    <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11"/>
+    <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12"/>
+    <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13"/>
+    <cfRule type="duplicateValues" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15"/>
+    <cfRule type="duplicateValues" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16"/>
+    <cfRule type="duplicateValues" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17"/>
+    <cfRule type="duplicateValues" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E8">
-    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18"/>
+    <cfRule type="duplicateValues" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19"/>
+    <cfRule type="duplicateValues" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20"/>
+    <cfRule type="duplicateValues" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21"/>
+    <cfRule type="duplicateValues" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22"/>
+    <cfRule type="duplicateValues" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8 E1:E2">
-    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23"/>
+    <cfRule type="duplicateValues" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8 E1:E4">
-    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24"/>
+    <cfRule type="duplicateValues" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:E1048576 C1:E1 C2 C8">
-    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25"/>
+    <cfRule type="duplicateValues" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:E1048576 C1:E1 C2:C4 C8">
-    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26"/>
+    <cfRule type="duplicateValues" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:E1048576 C8">
     <cfRule type="duplicateValues" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27"/>
@@ -2960,220 +2992,220 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="4" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="6" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>40</v>
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="13" t="n">
         <v>53000000</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>19</v>
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="13" t="n">
         <v>54000000</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="13" t="n">
         <v>55000000</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="13" t="n">
         <v>56000000</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="13" t="n">
         <v>57000000</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H7" s="13" t="n">
         <v>58000000</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>29</v>
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8" s="13" t="n">
         <v>59000000</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>32</v>
+      <c r="A9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -3182,18 +3214,18 @@
         <v>60000000</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>36</v>
+      <c r="A10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" s="19" t="n">
         <v>1401100404</v>
@@ -3205,7 +3237,7 @@
         <v>61000000</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3364,11 +3396,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="4" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="6" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17"/>
@@ -3377,83 +3409,83 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>40</v>
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="K1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="M1" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="Q1" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="R1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="T1" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
+      <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="13" t="n">
         <v>6500000</v>
       </c>
@@ -3493,25 +3525,25 @@
         <v>2200000</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>19</v>
+      <c r="A3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="13" t="n">
         <v>7000000</v>
       </c>
@@ -3551,25 +3583,25 @@
         <v>2300000</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="13" t="n">
         <v>7500000</v>
       </c>
@@ -3609,27 +3641,27 @@
         <v>2400000</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="13" t="n">
         <v>8000000</v>
       </c>
@@ -3669,27 +3701,27 @@
         <v>2500000</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="13" t="n">
         <v>8500000</v>
       </c>
@@ -3729,26 +3761,26 @@
         <v>2600000</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H7" s="13" t="n">
         <v>9000000</v>
@@ -3789,26 +3821,26 @@
         <v>2700000</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>29</v>
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H8" s="13" t="n">
         <v>9500000</v>
@@ -3849,21 +3881,21 @@
         <v>2800000</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>32</v>
+      <c r="A9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -3907,21 +3939,21 @@
         <v>2900000</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>36</v>
+      <c r="A10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="14"/>
@@ -3965,7 +3997,7 @@
         <v>3000000</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4128,103 +4160,103 @@
   <sheetData>
     <row r="1" s="34" customFormat="true" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M1" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P1" s="31" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R1" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T1" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U1" s="32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="V1" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W1" s="32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="X1" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Y1" s="30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
+      <c r="A2" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="35" t="n">
         <v>107759</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="25" t="n">
         <v>1200000</v>
       </c>
@@ -4271,31 +4303,31 @@
         <v>2600000</v>
       </c>
       <c r="Y2" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
+      <c r="A3" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="35" t="n">
         <v>107882</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>19</v>
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="25" t="n">
         <v>1300000</v>
       </c>
@@ -4342,31 +4374,31 @@
         <v>2700000</v>
       </c>
       <c r="Y3" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>21</v>
+      <c r="A4" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="35" t="n">
         <v>108005</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>23</v>
+        <v>84</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="25" t="n">
         <v>1400000</v>
       </c>
@@ -4413,31 +4445,31 @@
         <v>2800000</v>
       </c>
       <c r="Y4" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>25</v>
+      <c r="A5" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="35" t="n">
         <v>108128</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>27</v>
+        <v>85</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="25" t="n">
         <v>1500000</v>
       </c>
@@ -4484,27 +4516,27 @@
         <v>2900000</v>
       </c>
       <c r="Y5" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
+      <c r="A6" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="35" t="n">
         <v>108497</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>29</v>
+        <v>86</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -4555,27 +4587,27 @@
         <v>3000000</v>
       </c>
       <c r="Y6" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
+      <c r="A7" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="B7" s="35" t="n">
         <v>108620</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>87</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -4626,27 +4658,27 @@
         <v>3100000</v>
       </c>
       <c r="Y7" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>35</v>
+      <c r="A8" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B8" s="35" t="n">
         <v>108743</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>36</v>
+        <v>88</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="14"/>
@@ -4697,7 +4729,7 @@
         <v>3200000</v>
       </c>
       <c r="Y8" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4879,22 +4911,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="38" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G1" s="43" t="s">
         <v>2</v>
@@ -4908,19 +4940,19 @@
         <v>107759</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="F2" s="45" t="n">
         <v>3500000</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,19 +4963,19 @@
         <v>107882</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>19</v>
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="F3" s="45" t="n">
         <v>3600000</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,19 +4986,19 @@
         <v>108005</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>23</v>
+        <v>84</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="45" t="n">
         <v>3700000</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4977,19 +5009,19 @@
         <v>108128</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>27</v>
+        <v>85</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="45" t="n">
         <v>3800000</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5000,19 +5032,19 @@
         <v>108497</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>29</v>
+        <v>86</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="45" t="n">
         <v>3900000</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5023,19 +5055,19 @@
         <v>108620</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>87</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="45" t="n">
         <v>4000000</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>